<commit_message>
Finished Tests, made Graph w/ LOBF and function
</commit_message>
<xml_diff>
--- a/Excell Sheets/Disparity.xlsx
+++ b/Excell Sheets/Disparity.xlsx
@@ -19,18 +19,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Brightness</t>
   </si>
   <si>
     <t>Distance(mm)</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Brightness Average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -48,7 +57,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -118,11 +127,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -132,6 +156,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -147,6 +177,1695 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.9373113071758783E-2"/>
+          <c:y val="2.8259473346178548E-2"/>
+          <c:w val="0.71992667510104336"/>
+          <c:h val="0.85766652000869836"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Test 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2905</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1932</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1498</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1165</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>973</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>829</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>619</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>422</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>407</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>226</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5BED-4B71-83C2-74B338B4E41F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Test 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$23:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2954</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1959</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1489</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1186</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>974</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>839</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>619</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>547</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>396</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>356</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>322</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>184</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$23:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5BED-4B71-83C2-74B338B4E41F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Test 3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$42:$C$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2945</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1535</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1212</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>955</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>813</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>719</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>623</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>564</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>444</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>396</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>251</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$42:$B$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5BED-4B71-83C2-74B338B4E41F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Brightness Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.18974483137360015"/>
+                  <c:y val="-0.18608428281724901"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$4:$F$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2934.6666666666665</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1956.6666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1507.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1187.6666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>967.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>827</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>716.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>620.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>560.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>496.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>434</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>399.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>363.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>295.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>259.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>246.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>220.33333333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5BED-4B71-83C2-74B338B4E41F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="508263856"/>
+        <c:axId val="508265496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="508263856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t>Brightness values</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="508265496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="200"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="508265496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Distance (mm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="508263856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="200"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.82200617970821688"/>
+          <c:y val="0.39095170907104826"/>
+          <c:w val="0.17158456672375275"/>
+          <c:h val="0.21238480606590843"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -412,21 +2131,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D60"/>
+  <dimension ref="A2:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6" t="s">
         <v>1</v>
@@ -435,8 +2162,14 @@
         <v>0</v>
       </c>
       <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="1">
         <v>200</v>
@@ -445,8 +2178,15 @@
         <v>2905</v>
       </c>
       <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>200</v>
+      </c>
+      <c r="F4" s="10">
+        <f>(C4+C23+C42) / 3</f>
+        <v>2934.6666666666665</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="3">
         <v>300</v>
@@ -455,8 +2195,15 @@
         <v>1932</v>
       </c>
       <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="3">
+        <v>300</v>
+      </c>
+      <c r="F5" s="10">
+        <f>(C5+C24+C43) / 3</f>
+        <v>1956.6666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="3">
         <v>400</v>
@@ -465,8 +2212,15 @@
         <v>1498</v>
       </c>
       <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="3">
+        <v>400</v>
+      </c>
+      <c r="F6" s="10">
+        <f>(C6+C25+C44) / 3</f>
+        <v>1507.3333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="3">
         <v>500</v>
@@ -475,8 +2229,15 @@
         <v>1165</v>
       </c>
       <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="3">
+        <v>500</v>
+      </c>
+      <c r="F7" s="10">
+        <f>(C7+C26+C45) / 3</f>
+        <v>1187.6666666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="3">
         <v>600</v>
@@ -485,8 +2246,15 @@
         <v>973</v>
       </c>
       <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="3">
+        <v>600</v>
+      </c>
+      <c r="F8" s="10">
+        <f>(C8+C27+C46) / 3</f>
+        <v>967.33333333333337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="3">
         <v>700</v>
@@ -495,8 +2263,15 @@
         <v>829</v>
       </c>
       <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="3">
+        <v>700</v>
+      </c>
+      <c r="F9" s="10">
+        <f>(C9+C28+C47) / 3</f>
+        <v>827</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="3">
         <v>800</v>
@@ -505,8 +2280,15 @@
         <v>730</v>
       </c>
       <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="3">
+        <v>800</v>
+      </c>
+      <c r="F10" s="10">
+        <f>(C10+C29+C48) / 3</f>
+        <v>716.33333333333337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="3">
         <v>900</v>
@@ -515,8 +2297,15 @@
         <v>619</v>
       </c>
       <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="3">
+        <v>900</v>
+      </c>
+      <c r="F11" s="10">
+        <f>(C11+C30+C49) / 3</f>
+        <v>620.33333333333337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="3">
         <v>1000</v>
@@ -525,8 +2314,15 @@
         <v>570</v>
       </c>
       <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="3">
+        <v>1000</v>
+      </c>
+      <c r="F12" s="10">
+        <f>(C12+C31+C50) / 3</f>
+        <v>560.33333333333337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="3">
         <v>1100</v>
@@ -535,8 +2331,15 @@
         <v>504</v>
       </c>
       <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="3">
+        <v>1100</v>
+      </c>
+      <c r="F13" s="10">
+        <f>(C13+C32+C51) / 3</f>
+        <v>496.33333333333331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="3">
         <v>1200</v>
@@ -545,8 +2348,15 @@
         <v>422</v>
       </c>
       <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="3">
+        <v>1200</v>
+      </c>
+      <c r="F14" s="10">
+        <f>(C14+C33+C52) / 3</f>
+        <v>434</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="3">
         <v>1300</v>
@@ -555,8 +2365,15 @@
         <v>407</v>
       </c>
       <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="3">
+        <v>1300</v>
+      </c>
+      <c r="F15" s="10">
+        <f>(C15+C34+C53) / 3</f>
+        <v>399.66666666666669</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="3">
         <v>1400</v>
@@ -565,8 +2382,15 @@
         <v>375</v>
       </c>
       <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="3">
+        <v>1400</v>
+      </c>
+      <c r="F16" s="10">
+        <f>(C16+C35+C54) / 3</f>
+        <v>363.66666666666669</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="3">
         <v>1500</v>
@@ -575,8 +2399,15 @@
         <v>330</v>
       </c>
       <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="3">
+        <v>1500</v>
+      </c>
+      <c r="F17" s="10">
+        <f>(C17+C36+C55) / 3</f>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="3">
         <v>1600</v>
@@ -585,8 +2416,15 @@
         <v>299</v>
       </c>
       <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="3">
+        <v>1600</v>
+      </c>
+      <c r="F18" s="10">
+        <f>(C18+C37+C56) / 3</f>
+        <v>295.33333333333331</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="3">
         <v>1700</v>
@@ -595,8 +2433,15 @@
         <v>278</v>
       </c>
       <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="3">
+        <v>1700</v>
+      </c>
+      <c r="F19" s="10">
+        <f>(C19+C38+C57) / 3</f>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="3">
         <v>1800</v>
@@ -605,8 +2450,15 @@
         <v>264</v>
       </c>
       <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="3">
+        <v>1800</v>
+      </c>
+      <c r="F20" s="10">
+        <f>(C20+C39+C58) / 3</f>
+        <v>259.33333333333331</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="3">
         <v>1900</v>
@@ -615,8 +2467,15 @@
         <v>249</v>
       </c>
       <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="3">
+        <v>1900</v>
+      </c>
+      <c r="F21" s="10">
+        <f>(C21+C40+C59) / 3</f>
+        <v>246.66666666666666</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="5">
         <v>2000</v>
@@ -625,8 +2484,15 @@
         <v>226</v>
       </c>
       <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="5">
+        <v>2000</v>
+      </c>
+      <c r="F22" s="11">
+        <f>(C22+C41+C60) / 3</f>
+        <v>220.33333333333334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="1">
         <v>200</v>
@@ -636,7 +2502,7 @@
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="3">
         <v>300</v>
@@ -646,7 +2512,7 @@
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="3">
         <v>400</v>
@@ -656,7 +2522,7 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="3">
         <v>500</v>
@@ -666,7 +2532,7 @@
       </c>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="3">
         <v>600</v>
@@ -676,7 +2542,7 @@
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="3">
         <v>700</v>
@@ -686,7 +2552,7 @@
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="3">
         <v>800</v>
@@ -696,7 +2562,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="3">
         <v>900</v>
@@ -706,7 +2572,7 @@
       </c>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="3">
         <v>1000</v>
@@ -716,7 +2582,7 @@
       </c>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="3">
         <v>1100</v>
@@ -821,7 +2687,9 @@
       <c r="B42" s="1">
         <v>200</v>
       </c>
-      <c r="C42" s="7"/>
+      <c r="C42" s="7">
+        <v>2945</v>
+      </c>
       <c r="D42" s="6"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -829,7 +2697,9 @@
       <c r="B43" s="3">
         <v>300</v>
       </c>
-      <c r="C43" s="6"/>
+      <c r="C43" s="7">
+        <v>1979</v>
+      </c>
       <c r="D43" s="6"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -837,7 +2707,9 @@
       <c r="B44" s="3">
         <v>400</v>
       </c>
-      <c r="C44" s="6"/>
+      <c r="C44" s="7">
+        <v>1535</v>
+      </c>
       <c r="D44" s="6"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -845,85 +2717,137 @@
       <c r="B45" s="3">
         <v>500</v>
       </c>
-      <c r="C45" s="6"/>
+      <c r="C45" s="7">
+        <v>1212</v>
+      </c>
       <c r="D45" s="6"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
         <v>600</v>
       </c>
+      <c r="C46" s="7">
+        <v>955</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="3">
         <v>700</v>
       </c>
+      <c r="C47" s="7">
+        <v>813</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="3">
         <v>800</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C48" s="7">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="3">
         <v>900</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C49" s="7">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="7">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="3">
         <v>1100</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C51" s="7">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="3">
         <v>1200</v>
       </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C52" s="7">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="3">
         <v>1300</v>
       </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C53" s="7">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="3">
         <v>1400</v>
       </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C54" s="7">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="3">
         <v>1500</v>
       </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C55" s="7">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="3">
         <v>1600</v>
       </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C56" s="7">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="3">
         <v>1700</v>
       </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C57" s="7">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="3">
         <v>1800</v>
       </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C58" s="7">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="3">
         <v>1900</v>
       </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C59" s="7">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="5">
         <v>2000</v>
       </c>
+      <c r="C60" s="7">
+        <v>251</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Recorded 2nd set of data
Inaccuracies
</commit_message>
<xml_diff>
--- a/Excell Sheets/Disparity.xlsx
+++ b/Excell Sheets/Disparity.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Inaccuracies" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Brightness</t>
   </si>
@@ -31,6 +32,15 @@
   </si>
   <si>
     <t>Brightness Average</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Reported</t>
+  </si>
+  <si>
+    <t>tS: 12</t>
   </si>
 </sst>
 </file>
@@ -239,10 +249,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$22</c:f>
+              <c:f>Sheet1!$C$4:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2905</c:v>
                 </c:pt>
@@ -284,31 +294,16 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>330</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>299</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>278</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>264</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>249</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>226</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$22</c:f>
+              <c:f>Sheet1!$B$4:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>200</c:v>
                 </c:pt>
@@ -350,21 +345,6 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1600</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1900</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -406,10 +386,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$23:$C$41</c:f>
+              <c:f>Sheet1!$C$23:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2954</c:v>
                 </c:pt>
@@ -451,31 +431,16 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>322</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>277</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>248</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>224</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>208</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>184</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$23:$B$41</c:f>
+              <c:f>Sheet1!$B$23:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>200</c:v>
                 </c:pt>
@@ -517,21 +482,6 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1600</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1900</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -573,10 +523,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$42:$C$60</c:f>
+              <c:f>Sheet1!$C$42:$C$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2945</c:v>
                 </c:pt>
@@ -618,31 +568,16 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>338</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>310</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>293</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>283</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>251</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$42:$B$60</c:f>
+              <c:f>Sheet1!$B$42:$B$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>200</c:v>
                 </c:pt>
@@ -684,21 +619,6 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1600</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1900</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -762,8 +682,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.18974483137360015"/>
-                  <c:y val="-0.18608428281724901"/>
+                  <c:x val="0.20094641120554602"/>
+                  <c:y val="-0.15855263756770288"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -779,7 +699,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -798,10 +718,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$22</c:f>
+              <c:f>Sheet1!$F$4:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2934.6666666666665</c:v>
                 </c:pt>
@@ -843,31 +763,16 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>330</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>295.33333333333331</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>273</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>259.33333333333331</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>246.66666666666666</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>220.33333333333334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$4:$E$22</c:f>
+              <c:f>Sheet1!$E$4:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>200</c:v>
                 </c:pt>
@@ -909,21 +814,6 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1600</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1900</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1070,7 +960,7 @@
         <c:axId val="508265496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2200"/>
+          <c:max val="1800"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1206,9 +1096,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.82200617970821688"/>
-          <c:y val="0.39095170907104826"/>
+          <c:y val="0.25222338537162625"/>
           <c:w val="0.17158456672375275"/>
-          <c:h val="0.21238480606590843"/>
+          <c:h val="0.35111313397963984"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2133,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2850,4 +2740,356 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:E31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>200</v>
+      </c>
+      <c r="D4">
+        <v>205</v>
+      </c>
+      <c r="E4">
+        <v>3040</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>300</v>
+      </c>
+      <c r="D5">
+        <v>282</v>
+      </c>
+      <c r="E5">
+        <v>2151</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>400</v>
+      </c>
+      <c r="D6">
+        <v>384</v>
+      </c>
+      <c r="E6">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>479</v>
+      </c>
+      <c r="E7">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>600</v>
+      </c>
+      <c r="D8">
+        <v>579</v>
+      </c>
+      <c r="E8">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>700</v>
+      </c>
+      <c r="D9">
+        <v>672</v>
+      </c>
+      <c r="E9">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>800</v>
+      </c>
+      <c r="D10">
+        <v>759</v>
+      </c>
+      <c r="E10">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>900</v>
+      </c>
+      <c r="D11">
+        <v>809</v>
+      </c>
+      <c r="E11">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>1000</v>
+      </c>
+      <c r="D12">
+        <v>940</v>
+      </c>
+      <c r="E12">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>1100</v>
+      </c>
+      <c r="D13">
+        <v>1028</v>
+      </c>
+      <c r="E13">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>1200</v>
+      </c>
+      <c r="D14">
+        <v>1136</v>
+      </c>
+      <c r="E14">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>1300</v>
+      </c>
+      <c r="D15">
+        <v>1186</v>
+      </c>
+      <c r="E15">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>1400</v>
+      </c>
+      <c r="D16">
+        <v>1278</v>
+      </c>
+      <c r="E16">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>1500</v>
+      </c>
+      <c r="D17">
+        <v>1379</v>
+      </c>
+      <c r="E17">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>200</v>
+      </c>
+      <c r="D18">
+        <v>207</v>
+      </c>
+      <c r="E18">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>300</v>
+      </c>
+      <c r="D19">
+        <v>292</v>
+      </c>
+      <c r="E19">
+        <v>2071</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>400</v>
+      </c>
+      <c r="D20">
+        <v>380</v>
+      </c>
+      <c r="E20">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>500</v>
+      </c>
+      <c r="D21">
+        <v>484</v>
+      </c>
+      <c r="E21">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>600</v>
+      </c>
+      <c r="D22">
+        <v>578</v>
+      </c>
+      <c r="E22">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>700</v>
+      </c>
+      <c r="D23">
+        <v>653</v>
+      </c>
+      <c r="E23">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>800</v>
+      </c>
+      <c r="D24">
+        <v>760</v>
+      </c>
+      <c r="E24">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>900</v>
+      </c>
+      <c r="D25">
+        <v>841</v>
+      </c>
+      <c r="E25">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>1000</v>
+      </c>
+      <c r="D26">
+        <v>946</v>
+      </c>
+      <c r="E26">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>1100</v>
+      </c>
+      <c r="D27">
+        <v>1050</v>
+      </c>
+      <c r="E27">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>1200</v>
+      </c>
+      <c r="D28">
+        <v>1158</v>
+      </c>
+      <c r="E28">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>1300</v>
+      </c>
+      <c r="D29">
+        <v>1234</v>
+      </c>
+      <c r="E29">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>1400</v>
+      </c>
+      <c r="D30">
+        <v>1337</v>
+      </c>
+      <c r="E30">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>1500</v>
+      </c>
+      <c r="D31">
+        <v>1419</v>
+      </c>
+      <c r="E31">
+        <v>371</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Calculated average for inaccuracies
To be used in conjunction with the distance function.
</commit_message>
<xml_diff>
--- a/Excell Sheets/Disparity.xlsx
+++ b/Excell Sheets/Disparity.xlsx
@@ -166,12 +166,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -884,7 +884,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1009,7 +1008,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1167,7 +1165,1003 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Test 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Inaccuracies!$D$4:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>479</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>579</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>672</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>759</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>809</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1028</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1136</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1186</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1278</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1379</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Inaccuracies!$C$4:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-15E7-421A-8F43-4A022BA4CECD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Test 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Inaccuracies!$D$18:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>578</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>653</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>841</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>946</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1158</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1234</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1337</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1419</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Inaccuracies!$C$18:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-15E7-421A-8F43-4A022BA4CECD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Test 3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Inaccuracies!$D$32:$D$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>437</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>626</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>839</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>931</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1081</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1167</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1269</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1349</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Inaccuracies!$C$32:$C$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-15E7-421A-8F43-4A022BA4CECD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Tests average</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.32132531350247884"/>
+                  <c:y val="0.56018518518518523"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Inaccuracies!$I$4:$I$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>200.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>287.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>372.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>466.66666666666669</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>569</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>650.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>747</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>829.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>939</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1025.6666666666667</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1125</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1195.6666666666667</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1294.6666666666667</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1382.3333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Inaccuracies!$H$4:$H$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-15E7-421A-8F43-4A022BA4CECD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="485807152"/>
+        <c:axId val="485805840"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="485807152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Reported distance (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="485805840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="485805840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Actual</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> distance (mm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="485807152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.77503645377661123"/>
+          <c:y val="0.21672317002041416"/>
+          <c:w val="0.21755613881598135"/>
+          <c:h val="0.39062773403324585"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1723,6 +2717,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1737,6 +3247,41 @@
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2038,10 +3583,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="9"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
@@ -2055,7 +3600,7 @@
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2071,8 +3616,8 @@
       <c r="E4" s="1">
         <v>200</v>
       </c>
-      <c r="F4" s="10">
-        <f>(C4+C23+C42) / 3</f>
+      <c r="F4" s="9">
+        <f t="shared" ref="F4:F22" si="0">(C4+C23+C42) / 3</f>
         <v>2934.6666666666665</v>
       </c>
     </row>
@@ -2088,8 +3633,8 @@
       <c r="E5" s="3">
         <v>300</v>
       </c>
-      <c r="F5" s="10">
-        <f>(C5+C24+C43) / 3</f>
+      <c r="F5" s="9">
+        <f t="shared" si="0"/>
         <v>1956.6666666666667</v>
       </c>
     </row>
@@ -2105,8 +3650,8 @@
       <c r="E6" s="3">
         <v>400</v>
       </c>
-      <c r="F6" s="10">
-        <f>(C6+C25+C44) / 3</f>
+      <c r="F6" s="9">
+        <f t="shared" si="0"/>
         <v>1507.3333333333333</v>
       </c>
     </row>
@@ -2122,8 +3667,8 @@
       <c r="E7" s="3">
         <v>500</v>
       </c>
-      <c r="F7" s="10">
-        <f>(C7+C26+C45) / 3</f>
+      <c r="F7" s="9">
+        <f t="shared" si="0"/>
         <v>1187.6666666666667</v>
       </c>
     </row>
@@ -2139,8 +3684,8 @@
       <c r="E8" s="3">
         <v>600</v>
       </c>
-      <c r="F8" s="10">
-        <f>(C8+C27+C46) / 3</f>
+      <c r="F8" s="9">
+        <f t="shared" si="0"/>
         <v>967.33333333333337</v>
       </c>
     </row>
@@ -2156,8 +3701,8 @@
       <c r="E9" s="3">
         <v>700</v>
       </c>
-      <c r="F9" s="10">
-        <f>(C9+C28+C47) / 3</f>
+      <c r="F9" s="9">
+        <f t="shared" si="0"/>
         <v>827</v>
       </c>
     </row>
@@ -2173,8 +3718,8 @@
       <c r="E10" s="3">
         <v>800</v>
       </c>
-      <c r="F10" s="10">
-        <f>(C10+C29+C48) / 3</f>
+      <c r="F10" s="9">
+        <f t="shared" si="0"/>
         <v>716.33333333333337</v>
       </c>
     </row>
@@ -2190,8 +3735,8 @@
       <c r="E11" s="3">
         <v>900</v>
       </c>
-      <c r="F11" s="10">
-        <f>(C11+C30+C49) / 3</f>
+      <c r="F11" s="9">
+        <f t="shared" si="0"/>
         <v>620.33333333333337</v>
       </c>
     </row>
@@ -2207,8 +3752,8 @@
       <c r="E12" s="3">
         <v>1000</v>
       </c>
-      <c r="F12" s="10">
-        <f>(C12+C31+C50) / 3</f>
+      <c r="F12" s="9">
+        <f t="shared" si="0"/>
         <v>560.33333333333337</v>
       </c>
     </row>
@@ -2224,8 +3769,8 @@
       <c r="E13" s="3">
         <v>1100</v>
       </c>
-      <c r="F13" s="10">
-        <f>(C13+C32+C51) / 3</f>
+      <c r="F13" s="9">
+        <f t="shared" si="0"/>
         <v>496.33333333333331</v>
       </c>
     </row>
@@ -2241,8 +3786,8 @@
       <c r="E14" s="3">
         <v>1200</v>
       </c>
-      <c r="F14" s="10">
-        <f>(C14+C33+C52) / 3</f>
+      <c r="F14" s="9">
+        <f t="shared" si="0"/>
         <v>434</v>
       </c>
     </row>
@@ -2258,8 +3803,8 @@
       <c r="E15" s="3">
         <v>1300</v>
       </c>
-      <c r="F15" s="10">
-        <f>(C15+C34+C53) / 3</f>
+      <c r="F15" s="9">
+        <f t="shared" si="0"/>
         <v>399.66666666666669</v>
       </c>
     </row>
@@ -2275,8 +3820,8 @@
       <c r="E16" s="3">
         <v>1400</v>
       </c>
-      <c r="F16" s="10">
-        <f>(C16+C35+C54) / 3</f>
+      <c r="F16" s="9">
+        <f t="shared" si="0"/>
         <v>363.66666666666669</v>
       </c>
     </row>
@@ -2292,8 +3837,8 @@
       <c r="E17" s="3">
         <v>1500</v>
       </c>
-      <c r="F17" s="10">
-        <f>(C17+C36+C55) / 3</f>
+      <c r="F17" s="9">
+        <f t="shared" si="0"/>
         <v>330</v>
       </c>
     </row>
@@ -2309,8 +3854,8 @@
       <c r="E18" s="3">
         <v>1600</v>
       </c>
-      <c r="F18" s="10">
-        <f>(C18+C37+C56) / 3</f>
+      <c r="F18" s="9">
+        <f t="shared" si="0"/>
         <v>295.33333333333331</v>
       </c>
     </row>
@@ -2326,8 +3871,8 @@
       <c r="E19" s="3">
         <v>1700</v>
       </c>
-      <c r="F19" s="10">
-        <f>(C19+C38+C57) / 3</f>
+      <c r="F19" s="9">
+        <f t="shared" si="0"/>
         <v>273</v>
       </c>
     </row>
@@ -2343,8 +3888,8 @@
       <c r="E20" s="3">
         <v>1800</v>
       </c>
-      <c r="F20" s="10">
-        <f>(C20+C39+C58) / 3</f>
+      <c r="F20" s="9">
+        <f t="shared" si="0"/>
         <v>259.33333333333331</v>
       </c>
     </row>
@@ -2360,8 +3905,8 @@
       <c r="E21" s="3">
         <v>1900</v>
       </c>
-      <c r="F21" s="10">
-        <f>(C21+C40+C59) / 3</f>
+      <c r="F21" s="9">
+        <f t="shared" si="0"/>
         <v>246.66666666666666</v>
       </c>
     </row>
@@ -2377,8 +3922,8 @@
       <c r="E22" s="5">
         <v>2000</v>
       </c>
-      <c r="F22" s="11">
-        <f>(C22+C41+C60) / 3</f>
+      <c r="F22" s="10">
+        <f t="shared" si="0"/>
         <v>220.33333333333334</v>
       </c>
     </row>
@@ -2744,10 +4289,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:E31"/>
+  <dimension ref="C2:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,16 +4303,16 @@
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C2" s="9" t="s">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="12"/>
       <c r="E2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>4</v>
       </c>
@@ -2778,7 +4323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>200</v>
       </c>
@@ -2788,8 +4333,15 @@
       <c r="E4">
         <v>3040</v>
       </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>200</v>
+      </c>
+      <c r="I4">
+        <f>(D4+D18+D32) / 3</f>
+        <v>200.66666666666666</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>300</v>
       </c>
@@ -2799,8 +4351,15 @@
       <c r="E5">
         <v>2151</v>
       </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>300</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I17" si="0">(D5+D19+D33) / 3</f>
+        <v>287.66666666666669</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>400</v>
       </c>
@@ -2810,8 +4369,15 @@
       <c r="E6">
         <v>1533</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>400</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>372.33333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>500</v>
       </c>
@@ -2821,8 +4387,15 @@
       <c r="E7">
         <v>1208</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>500</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>466.66666666666669</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>600</v>
       </c>
@@ -2832,8 +4405,15 @@
       <c r="E8">
         <v>984</v>
       </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>600</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>569</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>700</v>
       </c>
@@ -2843,8 +4423,15 @@
       <c r="E9">
         <v>837</v>
       </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>700</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>650.33333333333337</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>800</v>
       </c>
@@ -2854,8 +4441,15 @@
       <c r="E10">
         <v>733</v>
       </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>800</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>747</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>900</v>
       </c>
@@ -2865,8 +4459,15 @@
       <c r="E11">
         <v>684</v>
       </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>900</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>829.66666666666663</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>1000</v>
       </c>
@@ -2876,8 +4477,15 @@
       <c r="E12">
         <v>586</v>
       </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>1000</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>939</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>1100</v>
       </c>
@@ -2887,8 +4495,15 @@
       <c r="E13">
         <v>527</v>
       </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>1100</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>1025.6666666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>1200</v>
       </c>
@@ -2898,8 +4513,15 @@
       <c r="E14">
         <v>473</v>
       </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>1200</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>1300</v>
       </c>
@@ -2909,8 +4531,15 @@
       <c r="E15">
         <v>451</v>
       </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>1300</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>1195.6666666666667</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>1400</v>
       </c>
@@ -2920,8 +4549,15 @@
       <c r="E16">
         <v>416</v>
       </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>1400</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>1294.6666666666667</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>1500</v>
       </c>
@@ -2931,8 +4567,15 @@
       <c r="E17">
         <v>383</v>
       </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>1500</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>1382.3333333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>200</v>
       </c>
@@ -2943,7 +4586,7 @@
         <v>3014</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>300</v>
       </c>
@@ -2954,7 +4597,7 @@
         <v>2071</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>400</v>
       </c>
@@ -2965,7 +4608,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>500</v>
       </c>
@@ -2976,7 +4619,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>600</v>
       </c>
@@ -2987,7 +4630,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>700</v>
       </c>
@@ -2998,7 +4641,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>800</v>
       </c>
@@ -3009,7 +4652,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>900</v>
       </c>
@@ -3020,7 +4663,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1000</v>
       </c>
@@ -3031,7 +4674,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>1100</v>
       </c>
@@ -3042,7 +4685,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>1200</v>
       </c>
@@ -3053,7 +4696,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>1300</v>
       </c>
@@ -3064,7 +4707,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>1400</v>
       </c>
@@ -3075,7 +4718,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>1500</v>
       </c>
@@ -3084,6 +4727,160 @@
       </c>
       <c r="E31">
         <v>371</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>200</v>
+      </c>
+      <c r="D32">
+        <v>190</v>
+      </c>
+      <c r="E32">
+        <v>3309</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>300</v>
+      </c>
+      <c r="D33">
+        <v>289</v>
+      </c>
+      <c r="E33">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>400</v>
+      </c>
+      <c r="D34">
+        <v>353</v>
+      </c>
+      <c r="E34">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>500</v>
+      </c>
+      <c r="D35">
+        <v>437</v>
+      </c>
+      <c r="E35">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>600</v>
+      </c>
+      <c r="D36">
+        <v>550</v>
+      </c>
+      <c r="E36">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>700</v>
+      </c>
+      <c r="D37">
+        <v>626</v>
+      </c>
+      <c r="E37">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>800</v>
+      </c>
+      <c r="D38">
+        <v>722</v>
+      </c>
+      <c r="E38">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>900</v>
+      </c>
+      <c r="D39">
+        <v>839</v>
+      </c>
+      <c r="E39">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>1000</v>
+      </c>
+      <c r="D40">
+        <v>931</v>
+      </c>
+      <c r="E40">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>1100</v>
+      </c>
+      <c r="D41">
+        <v>999</v>
+      </c>
+      <c r="E41">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>1200</v>
+      </c>
+      <c r="D42">
+        <v>1081</v>
+      </c>
+      <c r="E42">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>1300</v>
+      </c>
+      <c r="D43">
+        <v>1167</v>
+      </c>
+      <c r="E43">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>1400</v>
+      </c>
+      <c r="D44">
+        <v>1269</v>
+      </c>
+      <c r="E44">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>1500</v>
+      </c>
+      <c r="D45">
+        <v>1349</v>
+      </c>
+      <c r="E45">
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -3091,5 +4888,6 @@
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>